<commit_message>
step 08 with full dataset. + some refactoring of utils
</commit_message>
<xml_diff>
--- a/LookitLaughter.test/_LookitLaughter.test.xlsx
+++ b/LookitLaughter.test/_LookitLaughter.test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/47f02ae9a4562ecf/LegoGPI/babyjokes/LookitLaughter.test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{51460F77-7404-4413-A652-9875FCAE32C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{180F268E-4195-45F3-A968-9F32EB01FB37}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{51460F77-7404-4413-A652-9875FCAE32C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{013114D3-45CF-47D2-83BA-10467B036A91}"/>
   <bookViews>
-    <workbookView xWindow="1752" yWindow="3564" windowWidth="23040" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6105" yWindow="1560" windowWidth="43200" windowHeight="23445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -730,18 +730,19 @@
   <dimension ref="A1:U56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="T1" sqref="T1:T1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.109375" style="3"/>
+    <col min="16" max="16" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" style="3"/>
+    <col min="18" max="18" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -806,7 +807,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>92</v>
       </c>
@@ -865,7 +866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>93</v>
       </c>
@@ -924,7 +925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>94</v>
       </c>
@@ -983,7 +984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>95</v>
       </c>
@@ -1042,7 +1043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>96</v>
       </c>
@@ -1101,7 +1102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>97</v>
       </c>
@@ -1160,7 +1161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>98</v>
       </c>
@@ -1219,7 +1220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>99</v>
       </c>
@@ -1278,7 +1279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>100</v>
       </c>
@@ -1337,7 +1338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>101</v>
       </c>
@@ -1396,7 +1397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>102</v>
       </c>
@@ -1455,7 +1456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>103</v>
       </c>
@@ -1514,7 +1515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>104</v>
       </c>
@@ -1573,7 +1574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>105</v>
       </c>
@@ -1632,7 +1633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>57</v>
       </c>
@@ -1688,7 +1689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>58</v>
       </c>
@@ -1744,7 +1745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>59</v>
       </c>
@@ -1800,7 +1801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>60</v>
       </c>
@@ -1856,7 +1857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>61</v>
       </c>
@@ -1912,7 +1913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>62</v>
       </c>
@@ -1968,7 +1969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>63</v>
       </c>
@@ -2024,7 +2025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>64</v>
       </c>
@@ -2080,7 +2081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>65</v>
       </c>
@@ -2136,7 +2137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>66</v>
       </c>
@@ -2192,7 +2193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>67</v>
       </c>
@@ -2248,7 +2249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>68</v>
       </c>
@@ -2304,7 +2305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>69</v>
       </c>
@@ -2360,7 +2361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>70</v>
       </c>
@@ -2416,7 +2417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>71</v>
       </c>
@@ -2472,7 +2473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>76</v>
       </c>
@@ -2531,7 +2532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>77</v>
       </c>
@@ -2590,7 +2591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>78</v>
       </c>
@@ -2649,7 +2650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>79</v>
       </c>
@@ -2708,7 +2709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>80</v>
       </c>
@@ -2767,7 +2768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>81</v>
       </c>
@@ -2826,7 +2827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>82</v>
       </c>
@@ -2885,7 +2886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>83</v>
       </c>
@@ -2944,7 +2945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>84</v>
       </c>
@@ -3003,7 +3004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>85</v>
       </c>
@@ -3062,7 +3063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>86</v>
       </c>
@@ -3121,7 +3122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>87</v>
       </c>
@@ -3180,7 +3181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>88</v>
       </c>
@@ -3239,7 +3240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>30</v>
       </c>
@@ -3295,7 +3296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>31</v>
       </c>
@@ -3351,7 +3352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>33</v>
       </c>
@@ -3407,7 +3408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>35</v>
       </c>
@@ -3463,7 +3464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>36</v>
       </c>
@@ -3519,7 +3520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>37</v>
       </c>
@@ -3575,7 +3576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>39</v>
       </c>
@@ -3631,7 +3632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>40</v>
       </c>
@@ -3687,7 +3688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>42</v>
       </c>
@@ -3743,7 +3744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>43</v>
       </c>
@@ -3799,7 +3800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>44</v>
       </c>
@@ -3855,7 +3856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>46</v>
       </c>
@@ -3911,7 +3912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
add parent child location to excel
</commit_message>
<xml_diff>
--- a/LookitLaughter.test/_LookitLaughter.test.xlsx
+++ b/LookitLaughter.test/_LookitLaughter.test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/47f02ae9a4562ecf/LegoGPI/babyjokes/LookitLaughter.test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{51460F77-7404-4413-A652-9875FCAE32C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1105FD2A-442F-4C57-BE0F-076D4F79B376}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{51460F77-7404-4413-A652-9875FCAE32C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9FA34CF-7F6E-4F69-9FE8-938573CC8B6B}"/>
   <bookViews>
-    <workbookView xWindow="7185" yWindow="2835" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26895" yWindow="5295" windowWidth="29415" windowHeight="23445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="112">
   <si>
     <t>VideoID</t>
   </si>
@@ -353,6 +353,9 @@
   </si>
   <si>
     <t>LEFT</t>
+  </si>
+  <si>
+    <t>Child</t>
   </si>
 </sst>
 </file>
@@ -393,7 +396,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -416,12 +419,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -430,6 +444,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -737,10 +754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U56"/>
+  <dimension ref="A1:V56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1:U1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,7 +769,7 @@
     <col min="18" max="18" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -813,11 +830,14 @@
       <c r="T1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="V1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>91</v>
       </c>
@@ -876,10 +896,13 @@
         <v>1</v>
       </c>
       <c r="U2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="V2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>92</v>
       </c>
@@ -938,10 +961,13 @@
         <v>1</v>
       </c>
       <c r="U3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="V3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>93</v>
       </c>
@@ -1000,10 +1026,13 @@
         <v>1</v>
       </c>
       <c r="U4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="V4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>94</v>
       </c>
@@ -1062,10 +1091,13 @@
         <v>1</v>
       </c>
       <c r="U5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="V5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>95</v>
       </c>
@@ -1124,10 +1156,13 @@
         <v>1</v>
       </c>
       <c r="U6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="V6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>96</v>
       </c>
@@ -1186,10 +1221,13 @@
         <v>1</v>
       </c>
       <c r="U7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="V7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>97</v>
       </c>
@@ -1248,10 +1286,13 @@
         <v>1</v>
       </c>
       <c r="U8" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="V8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>98</v>
       </c>
@@ -1310,10 +1351,13 @@
         <v>1</v>
       </c>
       <c r="U9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="V9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>99</v>
       </c>
@@ -1372,10 +1416,13 @@
         <v>1</v>
       </c>
       <c r="U10" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="V10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>100</v>
       </c>
@@ -1434,10 +1481,13 @@
         <v>1</v>
       </c>
       <c r="U11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="V11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>101</v>
       </c>
@@ -1496,10 +1546,13 @@
         <v>1</v>
       </c>
       <c r="U12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="V12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>102</v>
       </c>
@@ -1558,10 +1611,13 @@
         <v>1</v>
       </c>
       <c r="U13" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="V13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>103</v>
       </c>
@@ -1620,10 +1676,13 @@
         <v>1</v>
       </c>
       <c r="U14" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="V14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>104</v>
       </c>
@@ -1682,10 +1741,13 @@
         <v>1</v>
       </c>
       <c r="U15" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="V15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -1744,10 +1806,13 @@
         <v>1</v>
       </c>
       <c r="U16" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -1806,10 +1871,13 @@
         <v>1</v>
       </c>
       <c r="U17" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V17" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -1868,10 +1936,13 @@
         <v>1</v>
       </c>
       <c r="U18" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -1930,10 +2001,13 @@
         <v>1</v>
       </c>
       <c r="U19" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V19" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>60</v>
       </c>
@@ -1992,10 +2066,13 @@
         <v>1</v>
       </c>
       <c r="U20" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>61</v>
       </c>
@@ -2054,10 +2131,13 @@
         <v>1</v>
       </c>
       <c r="U21" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>62</v>
       </c>
@@ -2116,10 +2196,13 @@
         <v>1</v>
       </c>
       <c r="U22" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V22" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -2178,10 +2261,13 @@
         <v>1</v>
       </c>
       <c r="U23" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V23" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>64</v>
       </c>
@@ -2240,10 +2326,13 @@
         <v>1</v>
       </c>
       <c r="U24" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V24" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>65</v>
       </c>
@@ -2302,10 +2391,13 @@
         <v>1</v>
       </c>
       <c r="U25" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V25" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>66</v>
       </c>
@@ -2364,10 +2456,13 @@
         <v>1</v>
       </c>
       <c r="U26" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V26" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>67</v>
       </c>
@@ -2426,10 +2521,13 @@
         <v>1</v>
       </c>
       <c r="U27" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V27" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>68</v>
       </c>
@@ -2488,10 +2586,13 @@
         <v>1</v>
       </c>
       <c r="U28" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V28" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>69</v>
       </c>
@@ -2550,10 +2651,13 @@
         <v>1</v>
       </c>
       <c r="U29" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V29" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>70</v>
       </c>
@@ -2612,10 +2716,13 @@
         <v>1</v>
       </c>
       <c r="U30" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V30" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>75</v>
       </c>
@@ -2674,10 +2781,13 @@
         <v>1</v>
       </c>
       <c r="U31" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V31" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>76</v>
       </c>
@@ -2736,10 +2846,13 @@
         <v>1</v>
       </c>
       <c r="U32" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V32" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>77</v>
       </c>
@@ -2798,10 +2911,13 @@
         <v>1</v>
       </c>
       <c r="U33" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V33" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>78</v>
       </c>
@@ -2860,10 +2976,13 @@
         <v>1</v>
       </c>
       <c r="U34" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V34" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>79</v>
       </c>
@@ -2922,10 +3041,13 @@
         <v>1</v>
       </c>
       <c r="U35" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V35" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>80</v>
       </c>
@@ -2984,10 +3106,13 @@
         <v>1</v>
       </c>
       <c r="U36" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V36" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>81</v>
       </c>
@@ -3046,10 +3171,13 @@
         <v>1</v>
       </c>
       <c r="U37" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V37" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>82</v>
       </c>
@@ -3108,10 +3236,13 @@
         <v>1</v>
       </c>
       <c r="U38" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V38" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>83</v>
       </c>
@@ -3170,10 +3301,13 @@
         <v>1</v>
       </c>
       <c r="U39" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V39" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>84</v>
       </c>
@@ -3232,10 +3366,13 @@
         <v>1</v>
       </c>
       <c r="U40" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V40" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>85</v>
       </c>
@@ -3294,10 +3431,13 @@
         <v>1</v>
       </c>
       <c r="U41" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V41" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>86</v>
       </c>
@@ -3356,10 +3496,13 @@
         <v>1</v>
       </c>
       <c r="U42" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V42" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>87</v>
       </c>
@@ -3418,10 +3561,13 @@
         <v>1</v>
       </c>
       <c r="U43" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V43" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>29</v>
       </c>
@@ -3480,10 +3626,13 @@
         <v>1</v>
       </c>
       <c r="U44" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V44" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>30</v>
       </c>
@@ -3542,10 +3691,13 @@
         <v>1</v>
       </c>
       <c r="U45" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V45" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>32</v>
       </c>
@@ -3604,10 +3756,13 @@
         <v>1</v>
       </c>
       <c r="U46" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V46" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>34</v>
       </c>
@@ -3666,10 +3821,13 @@
         <v>1</v>
       </c>
       <c r="U47" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V47" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>35</v>
       </c>
@@ -3728,10 +3886,13 @@
         <v>1</v>
       </c>
       <c r="U48" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V48" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>36</v>
       </c>
@@ -3790,10 +3951,13 @@
         <v>1</v>
       </c>
       <c r="U49" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V49" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>38</v>
       </c>
@@ -3852,10 +4016,13 @@
         <v>1</v>
       </c>
       <c r="U50" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V50" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>39</v>
       </c>
@@ -3914,10 +4081,13 @@
         <v>1</v>
       </c>
       <c r="U51" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V51" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>41</v>
       </c>
@@ -3976,10 +4146,13 @@
         <v>1</v>
       </c>
       <c r="U52" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V52" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>42</v>
       </c>
@@ -4038,10 +4211,13 @@
         <v>1</v>
       </c>
       <c r="U53" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V53" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>43</v>
       </c>
@@ -4100,10 +4276,13 @@
         <v>1</v>
       </c>
       <c r="U54" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V54" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>45</v>
       </c>
@@ -4162,10 +4341,13 @@
         <v>1</v>
       </c>
       <c r="U55" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="V55" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>46</v>
       </c>
@@ -4224,14 +4406,18 @@
         <v>1</v>
       </c>
       <c r="U56" t="s">
+        <v>109</v>
+      </c>
+      <c r="V56" t="s">
         <v>110</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U1440">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T1440">
     <sortCondition ref="L2:L1440"/>
     <sortCondition ref="A2:A1440"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Major upgrade Add utility functions for audio diarization, file I/O, keypoint processing, and video manipulation
- Implemented `diarization.py` for speaker diarization using PyAnnote.
- Created `io_utils.py` for handling file paths and processed videos data.
- Added `keypoint_utils.py` for keypoint normalization, filtering, and interpolation.
- Introduced `math_utils.py` for mathematical operations on keypoints and audio data.
- Developed `notebook_utils.py` for displaying configuration information in Jupyter notebooks.
- Implemented `speech.py` for audio transcription using OpenAI's Whisper model.
- Added `transform_utils.py` for coordinate transformations and bounding box conversions.
- Created `render.py` for visualizing annotated frames and rendering video outputs.
- Developed `video_utils.py` for creating annotated videos and adding audio tracks.
</commit_message>
<xml_diff>
--- a/LookitLaughter.test/_LookitLaughter.test.xlsx
+++ b/LookitLaughter.test/_LookitLaughter.test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/47f02ae9a4562ecf/LegoGPI/babyjokes/LookitLaughter.test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{51460F77-7404-4413-A652-9875FCAE32C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9FA34CF-7F6E-4F69-9FE8-938573CC8B6B}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{51460F77-7404-4413-A652-9875FCAE32C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F641303-43C2-4951-B9E0-C9BE9418F836}"/>
   <bookViews>
-    <workbookView xWindow="26895" yWindow="5295" windowWidth="29415" windowHeight="23445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7695" yWindow="9480" windowWidth="25950" windowHeight="19410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -109,60 +109,21 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>6c6MZQ.joke1.rep1.take1.ThatsNotAHat.mp4</t>
-  </si>
-  <si>
-    <t>6c6MZQ.joke1.rep2.take1.ThatsNotAHat.mp4</t>
-  </si>
-  <si>
     <t>Funny</t>
   </si>
   <si>
-    <t>6c6MZQ.joke1.rep3.take1.ThatsNotAHat.mp4</t>
-  </si>
-  <si>
     <t>NomNomNom</t>
   </si>
   <si>
-    <t>6c6MZQ.joke2.rep1.take1.NomNomNom.mp4</t>
-  </si>
-  <si>
-    <t>6c6MZQ.joke2.rep2.take1.NomNomNom.mp4</t>
-  </si>
-  <si>
-    <t>6c6MZQ.joke2.rep3.take1.NomNomNom.mp4</t>
-  </si>
-  <si>
     <t>Peekaboo</t>
   </si>
   <si>
-    <t>6c6MZQ.joke3.rep2.take1.Peekaboo.mp4</t>
-  </si>
-  <si>
-    <t>6c6MZQ.joke3.rep3.take1.Peekaboo.mp4</t>
-  </si>
-  <si>
     <t>ThatsNotACat</t>
   </si>
   <si>
-    <t>6c6MZQ.joke4.rep1.take1.ThatsNotACat.mp4</t>
-  </si>
-  <si>
-    <t>6c6MZQ.joke4.rep2.take1.ThatsNotACat.mp4</t>
-  </si>
-  <si>
-    <t>6c6MZQ.joke4.rep3.take1.ThatsNotACat.mp4</t>
-  </si>
-  <si>
     <t>TearingPaper</t>
   </si>
   <si>
-    <t>6c6MZQ.joke5.rep1.take1.TearingPaper.mp4</t>
-  </si>
-  <si>
-    <t>6c6MZQ.joke5.rep3.take1.TearingPaper.mp4</t>
-  </si>
-  <si>
     <t>38 weeks</t>
   </si>
   <si>
@@ -190,51 +151,6 @@
     <t>its not the normal games we play piper found some amusing and some she was just like what are you doing. the one with the stuffed animal, she doesnt know her animal sounds so she didnt really understand it was funny.</t>
   </si>
   <si>
-    <t>3dC3SQ.joke1.rep1.take1.TearingPaper.mp4</t>
-  </si>
-  <si>
-    <t>3dC3SQ.joke1.rep2.take1.TearingPaper.mp4</t>
-  </si>
-  <si>
-    <t>3dC3SQ.joke1.rep3.take1.TearingPaper.mp4</t>
-  </si>
-  <si>
-    <t>3dC3SQ.joke2.rep1.take1.Peekaboo.mp4</t>
-  </si>
-  <si>
-    <t>3dC3SQ.joke2.rep2.take1.Peekaboo.mp4</t>
-  </si>
-  <si>
-    <t>3dC3SQ.joke2.rep3.take1.Peekaboo.mp4</t>
-  </si>
-  <si>
-    <t>3dC3SQ.joke3.rep1.take1.ThatsNotACat.mp4</t>
-  </si>
-  <si>
-    <t>3dC3SQ.joke3.rep2.take1.ThatsNotACat.mp4</t>
-  </si>
-  <si>
-    <t>3dC3SQ.joke3.rep3.take1.ThatsNotACat.mp4</t>
-  </si>
-  <si>
-    <t>3dC3SQ.joke4.rep1.take1.ThatsNotAHat.mp4</t>
-  </si>
-  <si>
-    <t>3dC3SQ.joke4.rep2.take1.ThatsNotAHat.mp4</t>
-  </si>
-  <si>
-    <t>3dC3SQ.joke4.rep3.take1.ThatsNotAHat.mp4</t>
-  </si>
-  <si>
-    <t>3dC3SQ.joke5.rep1.take1.NomNomNom.mp4</t>
-  </si>
-  <si>
-    <t>3dC3SQ.joke5.rep2.take1.NomNomNom.mp4</t>
-  </si>
-  <si>
-    <t>3dC3SQ.joke5.rep3.take1.NomNomNom.mp4</t>
-  </si>
-  <si>
     <t>['NomNomNom', 'ThatsNotAHat', 'Peekaboo', 'ThatsNotACat', 'TearingPaper']</t>
   </si>
   <si>
@@ -247,45 +163,6 @@
     <t>4JDccE</t>
   </si>
   <si>
-    <t>4JDccE.joke1.rep1.take1.NomNomNom.mp4</t>
-  </si>
-  <si>
-    <t>4JDccE.joke1.rep2.take1.NomNomNom.mp4</t>
-  </si>
-  <si>
-    <t>4JDccE.joke1.rep3.take1.NomNomNom.mp4</t>
-  </si>
-  <si>
-    <t>4JDccE.joke2.rep1.take1.ThatsNotAHat.mp4</t>
-  </si>
-  <si>
-    <t>4JDccE.joke2.rep2.take1.ThatsNotAHat.mp4</t>
-  </si>
-  <si>
-    <t>4JDccE.joke2.rep3.take1.ThatsNotAHat.mp4</t>
-  </si>
-  <si>
-    <t>4JDccE.joke3.rep2.take1.Peekaboo.mp4</t>
-  </si>
-  <si>
-    <t>4JDccE.joke3.rep3.take1.Peekaboo.mp4</t>
-  </si>
-  <si>
-    <t>4JDccE.joke4.rep1.take1.ThatsNotACat.mp4</t>
-  </si>
-  <si>
-    <t>4JDccE.joke4.rep3.take1.ThatsNotACat.mp4</t>
-  </si>
-  <si>
-    <t>4JDccE.joke5.rep1.take1.TearingPaper.mp4</t>
-  </si>
-  <si>
-    <t>4JDccE.joke5.rep2.take1.TearingPaper.mp4</t>
-  </si>
-  <si>
-    <t>4JDccE.joke5.rep3.take1.TearingPaper.mp4</t>
-  </si>
-  <si>
     <t>5ZQUSU</t>
   </si>
   <si>
@@ -295,48 +172,6 @@
     <t>['Peekaboo', 'NomNomNom', 'ThatsNotAHat', 'TearingPaper', 'ThatsNotACat']</t>
   </si>
   <si>
-    <t>2UWdXP.joke1.rep2.take1.Peekaboo.mp4</t>
-  </si>
-  <si>
-    <t>2UWdXP.joke1.rep3.take1.Peekaboo.mp4</t>
-  </si>
-  <si>
-    <t>2UWdXP.joke2.rep1.take1.NomNomNom.mp4</t>
-  </si>
-  <si>
-    <t>2UWdXP.joke2.rep2.take1.NomNomNom.mp4</t>
-  </si>
-  <si>
-    <t>2UWdXP.joke2.rep3.take1.NomNomNom.mp4</t>
-  </si>
-  <si>
-    <t>2UWdXP.joke3.rep1.take1.ThatsNotAHat.mp4</t>
-  </si>
-  <si>
-    <t>2UWdXP.joke3.rep2.take1.ThatsNotAHat.mp4</t>
-  </si>
-  <si>
-    <t>2UWdXP.joke3.rep3.take1.ThatsNotAHat.mp4</t>
-  </si>
-  <si>
-    <t>2UWdXP.joke4.rep1.take1.TearingPaper.mp4</t>
-  </si>
-  <si>
-    <t>2UWdXP.joke4.rep2.take1.TearingPaper.mp4</t>
-  </si>
-  <si>
-    <t>2UWdXP.joke4.rep3.take1.TearingPaper.mp4</t>
-  </si>
-  <si>
-    <t>2UWdXP.joke5.rep1.take1.ThatsNotACat.mp4</t>
-  </si>
-  <si>
-    <t>2UWdXP.joke5.rep2.take1.ThatsNotACat.mp4</t>
-  </si>
-  <si>
-    <t>2UWdXP.joke5.rep3.take1.ThatsNotACat.mp4</t>
-  </si>
-  <si>
     <t>JokeTake</t>
   </si>
   <si>
@@ -356,6 +191,171 @@
   </si>
   <si>
     <t>Child</t>
+  </si>
+  <si>
+    <t>2UWdXP.joke1.rep2.take1.Peekaboo_h265.mp4</t>
+  </si>
+  <si>
+    <t>2UWdXP.joke1.rep3.take1.Peekaboo_h265.mp4</t>
+  </si>
+  <si>
+    <t>2UWdXP.joke2.rep1.take1.NomNomNom_h265.mp4</t>
+  </si>
+  <si>
+    <t>2UWdXP.joke2.rep2.take1.NomNomNom_h265.mp4</t>
+  </si>
+  <si>
+    <t>2UWdXP.joke2.rep3.take1.NomNomNom_h265.mp4</t>
+  </si>
+  <si>
+    <t>2UWdXP.joke3.rep1.take1.ThatsNotAHat_h265.mp4</t>
+  </si>
+  <si>
+    <t>2UWdXP.joke3.rep2.take1.ThatsNotAHat_h265.mp4</t>
+  </si>
+  <si>
+    <t>2UWdXP.joke3.rep3.take1.ThatsNotAHat_h265.mp4</t>
+  </si>
+  <si>
+    <t>2UWdXP.joke4.rep1.take1.TearingPaper_h265.mp4</t>
+  </si>
+  <si>
+    <t>2UWdXP.joke4.rep2.take1.TearingPaper_h265.mp4</t>
+  </si>
+  <si>
+    <t>2UWdXP.joke4.rep3.take1.TearingPaper_h265.mp4</t>
+  </si>
+  <si>
+    <t>2UWdXP.joke5.rep1.take1.ThatsNotACat_h265.mp4</t>
+  </si>
+  <si>
+    <t>2UWdXP.joke5.rep2.take1.ThatsNotACat_h265.mp4</t>
+  </si>
+  <si>
+    <t>2UWdXP.joke5.rep3.take1.ThatsNotACat_h265.mp4</t>
+  </si>
+  <si>
+    <t>3dC3SQ.joke1.rep1.take1.TearingPaper_h265.mp4</t>
+  </si>
+  <si>
+    <t>3dC3SQ.joke1.rep2.take1.TearingPaper_h265.mp4</t>
+  </si>
+  <si>
+    <t>3dC3SQ.joke1.rep3.take1.TearingPaper_h265.mp4</t>
+  </si>
+  <si>
+    <t>3dC3SQ.joke2.rep1.take1.Peekaboo_h265.mp4</t>
+  </si>
+  <si>
+    <t>3dC3SQ.joke2.rep2.take1.Peekaboo_h265.mp4</t>
+  </si>
+  <si>
+    <t>3dC3SQ.joke2.rep3.take1.Peekaboo_h265.mp4</t>
+  </si>
+  <si>
+    <t>3dC3SQ.joke3.rep1.take1.ThatsNotACat_h265.mp4</t>
+  </si>
+  <si>
+    <t>3dC3SQ.joke3.rep2.take1.ThatsNotACat_h265.mp4</t>
+  </si>
+  <si>
+    <t>3dC3SQ.joke3.rep3.take1.ThatsNotACat_h265.mp4</t>
+  </si>
+  <si>
+    <t>3dC3SQ.joke4.rep1.take1.ThatsNotAHat_h265.mp4</t>
+  </si>
+  <si>
+    <t>3dC3SQ.joke4.rep2.take1.ThatsNotAHat_h265.mp4</t>
+  </si>
+  <si>
+    <t>3dC3SQ.joke4.rep3.take1.ThatsNotAHat_h265.mp4</t>
+  </si>
+  <si>
+    <t>3dC3SQ.joke5.rep1.take1.NomNomNom_h265.mp4</t>
+  </si>
+  <si>
+    <t>3dC3SQ.joke5.rep2.take1.NomNomNom_h265.mp4</t>
+  </si>
+  <si>
+    <t>3dC3SQ.joke5.rep3.take1.NomNomNom_h265.mp4</t>
+  </si>
+  <si>
+    <t>4JDccE.joke1.rep1.take1.NomNomNom_h265.mp4</t>
+  </si>
+  <si>
+    <t>4JDccE.joke1.rep2.take1.NomNomNom_h265.mp4</t>
+  </si>
+  <si>
+    <t>4JDccE.joke1.rep3.take1.NomNomNom_h265.mp4</t>
+  </si>
+  <si>
+    <t>4JDccE.joke2.rep1.take1.ThatsNotAHat_h265.mp4</t>
+  </si>
+  <si>
+    <t>4JDccE.joke2.rep2.take1.ThatsNotAHat_h265.mp4</t>
+  </si>
+  <si>
+    <t>4JDccE.joke2.rep3.take1.ThatsNotAHat_h265.mp4</t>
+  </si>
+  <si>
+    <t>4JDccE.joke3.rep2.take1.Peekaboo_h265.mp4</t>
+  </si>
+  <si>
+    <t>4JDccE.joke3.rep3.take1.Peekaboo_h265.mp4</t>
+  </si>
+  <si>
+    <t>4JDccE.joke4.rep1.take1.ThatsNotACat_h265.mp4</t>
+  </si>
+  <si>
+    <t>4JDccE.joke4.rep3.take1.ThatsNotACat_h265.mp4</t>
+  </si>
+  <si>
+    <t>4JDccE.joke5.rep1.take1.TearingPaper_h265.mp4</t>
+  </si>
+  <si>
+    <t>4JDccE.joke5.rep2.take1.TearingPaper_h265.mp4</t>
+  </si>
+  <si>
+    <t>4JDccE.joke5.rep3.take1.TearingPaper_h265.mp4</t>
+  </si>
+  <si>
+    <t>6c6MZQ.joke1.rep1.take1.ThatsNotAHat_h265.mp4</t>
+  </si>
+  <si>
+    <t>6c6MZQ.joke1.rep2.take1.ThatsNotAHat_h265.mp4</t>
+  </si>
+  <si>
+    <t>6c6MZQ.joke1.rep3.take1.ThatsNotAHat_h265.mp4</t>
+  </si>
+  <si>
+    <t>6c6MZQ.joke2.rep1.take1.NomNomNom_h265.mp4</t>
+  </si>
+  <si>
+    <t>6c6MZQ.joke2.rep2.take1.NomNomNom_h265.mp4</t>
+  </si>
+  <si>
+    <t>6c6MZQ.joke2.rep3.take1.NomNomNom_h265.mp4</t>
+  </si>
+  <si>
+    <t>6c6MZQ.joke3.rep2.take1.Peekaboo_h265.mp4</t>
+  </si>
+  <si>
+    <t>6c6MZQ.joke3.rep3.take1.Peekaboo_h265.mp4</t>
+  </si>
+  <si>
+    <t>6c6MZQ.joke4.rep1.take1.ThatsNotACat_h265.mp4</t>
+  </si>
+  <si>
+    <t>6c6MZQ.joke4.rep2.take1.ThatsNotACat_h265.mp4</t>
+  </si>
+  <si>
+    <t>6c6MZQ.joke4.rep3.take1.ThatsNotACat_h265.mp4</t>
+  </si>
+  <si>
+    <t>6c6MZQ.joke5.rep1.take1.TearingPaper_h265.mp4</t>
+  </si>
+  <si>
+    <t>6c6MZQ.joke5.rep3.take1.TearingPaper_h265.mp4</t>
   </si>
 </sst>
 </file>
@@ -444,7 +444,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -756,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:U1048576"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AJ10" sqref="AJ10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,27 +819,27 @@
         <v>16</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>107</v>
+        <v>52</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>106</v>
+        <v>51</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>105</v>
+        <v>50</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>111</v>
+        <v>56</v>
       </c>
       <c r="V1" t="s">
-        <v>108</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
@@ -848,10 +848,10 @@
         <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="E2" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="F2">
         <v>233</v>
@@ -860,13 +860,13 @@
         <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="I2" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="J2" t="s">
-        <v>90</v>
+        <v>49</v>
       </c>
       <c r="L2" t="s">
         <v>24</v>
@@ -878,13 +878,13 @@
         <v>25</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>27</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="R2">
         <v>1</v>
@@ -896,15 +896,15 @@
         <v>1</v>
       </c>
       <c r="U2" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
       <c r="V2" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
@@ -913,10 +913,10 @@
         <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="E3" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="F3">
         <v>233</v>
@@ -925,13 +925,13 @@
         <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="I3" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="J3" t="s">
-        <v>90</v>
+        <v>49</v>
       </c>
       <c r="L3" t="s">
         <v>24</v>
@@ -943,13 +943,13 @@
         <v>25</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="P3" s="3" t="s">
         <v>27</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="R3">
         <v>1</v>
@@ -961,15 +961,15 @@
         <v>1</v>
       </c>
       <c r="U3" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
       <c r="V3" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
         <v>17</v>
@@ -978,10 +978,10 @@
         <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="E4" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="F4">
         <v>233</v>
@@ -990,13 +990,13 @@
         <v>20</v>
       </c>
       <c r="H4" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="I4" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="J4" t="s">
-        <v>90</v>
+        <v>49</v>
       </c>
       <c r="L4" t="s">
         <v>24</v>
@@ -1008,13 +1008,13 @@
         <v>25</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="R4">
         <v>2</v>
@@ -1026,15 +1026,15 @@
         <v>1</v>
       </c>
       <c r="U4" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
       <c r="V4" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
@@ -1043,10 +1043,10 @@
         <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="E5" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="F5">
         <v>233</v>
@@ -1055,13 +1055,13 @@
         <v>20</v>
       </c>
       <c r="H5" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="I5" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="J5" t="s">
-        <v>90</v>
+        <v>49</v>
       </c>
       <c r="L5" t="s">
         <v>24</v>
@@ -1073,13 +1073,13 @@
         <v>25</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="P5" s="3" t="s">
         <v>27</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="R5">
         <v>2</v>
@@ -1091,15 +1091,15 @@
         <v>1</v>
       </c>
       <c r="U5" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
       <c r="V5" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
@@ -1108,10 +1108,10 @@
         <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="E6" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="F6">
         <v>233</v>
@@ -1120,13 +1120,13 @@
         <v>20</v>
       </c>
       <c r="H6" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="I6" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="J6" t="s">
-        <v>90</v>
+        <v>49</v>
       </c>
       <c r="L6" t="s">
         <v>24</v>
@@ -1138,13 +1138,13 @@
         <v>25</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="P6" s="3" t="s">
         <v>27</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="R6">
         <v>2</v>
@@ -1156,15 +1156,15 @@
         <v>1</v>
       </c>
       <c r="U6" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
       <c r="V6" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>62</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
@@ -1173,10 +1173,10 @@
         <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="E7" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="F7">
         <v>233</v>
@@ -1185,13 +1185,13 @@
         <v>20</v>
       </c>
       <c r="H7" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="I7" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="J7" t="s">
-        <v>90</v>
+        <v>49</v>
       </c>
       <c r="L7" t="s">
         <v>24</v>
@@ -1206,10 +1206,10 @@
         <v>26</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="R7">
         <v>3</v>
@@ -1221,15 +1221,15 @@
         <v>1</v>
       </c>
       <c r="U7" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
       <c r="V7" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>97</v>
+        <v>63</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
@@ -1238,10 +1238,10 @@
         <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="F8">
         <v>233</v>
@@ -1250,13 +1250,13 @@
         <v>20</v>
       </c>
       <c r="H8" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="I8" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="J8" t="s">
-        <v>90</v>
+        <v>49</v>
       </c>
       <c r="L8" t="s">
         <v>24</v>
@@ -1271,10 +1271,10 @@
         <v>26</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="R8">
         <v>3</v>
@@ -1286,15 +1286,15 @@
         <v>1</v>
       </c>
       <c r="U8" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
       <c r="V8" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
@@ -1303,10 +1303,10 @@
         <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="E9" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="F9">
         <v>233</v>
@@ -1315,13 +1315,13 @@
         <v>20</v>
       </c>
       <c r="H9" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="I9" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="J9" t="s">
-        <v>90</v>
+        <v>49</v>
       </c>
       <c r="L9" t="s">
         <v>24</v>
@@ -1336,10 +1336,10 @@
         <v>26</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="R9">
         <v>3</v>
@@ -1351,15 +1351,15 @@
         <v>1</v>
       </c>
       <c r="U9" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
       <c r="V9" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>65</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
@@ -1368,10 +1368,10 @@
         <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="E10" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="F10">
         <v>233</v>
@@ -1380,13 +1380,13 @@
         <v>20</v>
       </c>
       <c r="H10" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="I10" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="J10" t="s">
-        <v>90</v>
+        <v>49</v>
       </c>
       <c r="L10" t="s">
         <v>24</v>
@@ -1398,13 +1398,13 @@
         <v>25</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="R10">
         <v>4</v>
@@ -1416,15 +1416,15 @@
         <v>1</v>
       </c>
       <c r="U10" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
       <c r="V10" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>100</v>
+        <v>66</v>
       </c>
       <c r="B11" t="s">
         <v>17</v>
@@ -1433,10 +1433,10 @@
         <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="E11" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="F11">
         <v>233</v>
@@ -1445,13 +1445,13 @@
         <v>20</v>
       </c>
       <c r="H11" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="I11" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="J11" t="s">
-        <v>90</v>
+        <v>49</v>
       </c>
       <c r="L11" t="s">
         <v>24</v>
@@ -1463,13 +1463,13 @@
         <v>25</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="R11">
         <v>4</v>
@@ -1481,15 +1481,15 @@
         <v>1</v>
       </c>
       <c r="U11" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
       <c r="V11" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>101</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
         <v>17</v>
@@ -1498,10 +1498,10 @@
         <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="E12" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="F12">
         <v>233</v>
@@ -1510,13 +1510,13 @@
         <v>20</v>
       </c>
       <c r="H12" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="I12" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="J12" t="s">
-        <v>90</v>
+        <v>49</v>
       </c>
       <c r="L12" t="s">
         <v>24</v>
@@ -1528,13 +1528,13 @@
         <v>25</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="R12">
         <v>4</v>
@@ -1546,15 +1546,15 @@
         <v>1</v>
       </c>
       <c r="U12" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
       <c r="V12" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="B13" t="s">
         <v>17</v>
@@ -1563,10 +1563,10 @@
         <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="E13" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="F13">
         <v>233</v>
@@ -1575,13 +1575,13 @@
         <v>20</v>
       </c>
       <c r="H13" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="I13" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="J13" t="s">
-        <v>90</v>
+        <v>49</v>
       </c>
       <c r="L13" t="s">
         <v>24</v>
@@ -1593,13 +1593,13 @@
         <v>25</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="P13" s="3" t="s">
         <v>27</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="R13">
         <v>5</v>
@@ -1611,15 +1611,15 @@
         <v>1</v>
       </c>
       <c r="U13" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
       <c r="V13" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>103</v>
+        <v>69</v>
       </c>
       <c r="B14" t="s">
         <v>17</v>
@@ -1628,10 +1628,10 @@
         <v>24</v>
       </c>
       <c r="D14" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="E14" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="F14">
         <v>233</v>
@@ -1640,13 +1640,13 @@
         <v>20</v>
       </c>
       <c r="H14" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="I14" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="J14" t="s">
-        <v>90</v>
+        <v>49</v>
       </c>
       <c r="L14" t="s">
         <v>24</v>
@@ -1658,13 +1658,13 @@
         <v>25</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="R14">
         <v>5</v>
@@ -1676,15 +1676,15 @@
         <v>1</v>
       </c>
       <c r="U14" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
       <c r="V14" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>104</v>
+        <v>70</v>
       </c>
       <c r="B15" t="s">
         <v>17</v>
@@ -1693,10 +1693,10 @@
         <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="E15" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="F15">
         <v>233</v>
@@ -1705,13 +1705,13 @@
         <v>20</v>
       </c>
       <c r="H15" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="I15" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="J15" t="s">
-        <v>90</v>
+        <v>49</v>
       </c>
       <c r="L15" t="s">
         <v>24</v>
@@ -1723,13 +1723,13 @@
         <v>25</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="R15">
         <v>5</v>
@@ -1741,15 +1741,15 @@
         <v>1</v>
       </c>
       <c r="U15" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
       <c r="V15" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
@@ -1758,10 +1758,10 @@
         <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E16" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F16">
         <v>780</v>
@@ -1773,10 +1773,10 @@
         <v>21</v>
       </c>
       <c r="J16" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="K16" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="L16" t="s">
         <v>24</v>
@@ -1788,13 +1788,13 @@
         <v>25</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="P16" s="3" t="s">
         <v>27</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="R16">
         <v>1</v>
@@ -1806,15 +1806,15 @@
         <v>1</v>
       </c>
       <c r="U16" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V16" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
@@ -1823,10 +1823,10 @@
         <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E17" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F17">
         <v>780</v>
@@ -1838,10 +1838,10 @@
         <v>21</v>
       </c>
       <c r="J17" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="K17" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="L17" t="s">
         <v>24</v>
@@ -1853,7 +1853,7 @@
         <v>25</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="P17" s="3" t="s">
         <v>27</v>
@@ -1871,15 +1871,15 @@
         <v>1</v>
       </c>
       <c r="U17" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V17" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
@@ -1888,10 +1888,10 @@
         <v>24</v>
       </c>
       <c r="D18" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E18" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F18">
         <v>780</v>
@@ -1903,10 +1903,10 @@
         <v>21</v>
       </c>
       <c r="J18" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="K18" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="L18" t="s">
         <v>24</v>
@@ -1918,10 +1918,10 @@
         <v>25</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Q18" s="3" t="s">
         <v>28</v>
@@ -1936,15 +1936,15 @@
         <v>1</v>
       </c>
       <c r="U18" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V18" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="B19" t="s">
         <v>17</v>
@@ -1953,10 +1953,10 @@
         <v>24</v>
       </c>
       <c r="D19" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E19" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F19">
         <v>780</v>
@@ -1968,10 +1968,10 @@
         <v>21</v>
       </c>
       <c r="J19" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="K19" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="L19" t="s">
         <v>24</v>
@@ -1983,7 +1983,7 @@
         <v>25</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="P19" s="3" t="s">
         <v>27</v>
@@ -2001,15 +2001,15 @@
         <v>1</v>
       </c>
       <c r="U19" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V19" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="B20" t="s">
         <v>17</v>
@@ -2018,10 +2018,10 @@
         <v>24</v>
       </c>
       <c r="D20" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E20" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F20">
         <v>780</v>
@@ -2033,10 +2033,10 @@
         <v>21</v>
       </c>
       <c r="J20" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="K20" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="L20" t="s">
         <v>24</v>
@@ -2048,10 +2048,10 @@
         <v>25</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="P20" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Q20" s="3" t="s">
         <v>28</v>
@@ -2066,15 +2066,15 @@
         <v>1</v>
       </c>
       <c r="U20" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V20" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="B21" t="s">
         <v>17</v>
@@ -2083,10 +2083,10 @@
         <v>24</v>
       </c>
       <c r="D21" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E21" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F21">
         <v>780</v>
@@ -2098,10 +2098,10 @@
         <v>21</v>
       </c>
       <c r="J21" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="K21" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="L21" t="s">
         <v>24</v>
@@ -2113,7 +2113,7 @@
         <v>25</v>
       </c>
       <c r="O21" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="P21" s="3" t="s">
         <v>27</v>
@@ -2131,15 +2131,15 @@
         <v>1</v>
       </c>
       <c r="U21" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V21" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="B22" t="s">
         <v>17</v>
@@ -2148,10 +2148,10 @@
         <v>24</v>
       </c>
       <c r="D22" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E22" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F22">
         <v>780</v>
@@ -2163,10 +2163,10 @@
         <v>21</v>
       </c>
       <c r="J22" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="K22" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="L22" t="s">
         <v>24</v>
@@ -2178,13 +2178,13 @@
         <v>25</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="P22" s="3" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="R22">
         <v>3</v>
@@ -2196,15 +2196,15 @@
         <v>1</v>
       </c>
       <c r="U22" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V22" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
         <v>17</v>
@@ -2213,10 +2213,10 @@
         <v>24</v>
       </c>
       <c r="D23" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E23" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F23">
         <v>780</v>
@@ -2228,10 +2228,10 @@
         <v>21</v>
       </c>
       <c r="J23" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="K23" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="L23" t="s">
         <v>24</v>
@@ -2243,10 +2243,10 @@
         <v>25</v>
       </c>
       <c r="O23" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="P23" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Q23" s="3" t="s">
         <v>28</v>
@@ -2261,15 +2261,15 @@
         <v>1</v>
       </c>
       <c r="U23" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V23" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="B24" t="s">
         <v>17</v>
@@ -2278,10 +2278,10 @@
         <v>24</v>
       </c>
       <c r="D24" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E24" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F24">
         <v>780</v>
@@ -2293,10 +2293,10 @@
         <v>21</v>
       </c>
       <c r="J24" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="K24" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="L24" t="s">
         <v>24</v>
@@ -2308,13 +2308,13 @@
         <v>25</v>
       </c>
       <c r="O24" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="P24" s="3" t="s">
         <v>27</v>
       </c>
       <c r="Q24" s="3" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="R24">
         <v>3</v>
@@ -2326,15 +2326,15 @@
         <v>1</v>
       </c>
       <c r="U24" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V24" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="B25" t="s">
         <v>17</v>
@@ -2343,10 +2343,10 @@
         <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E25" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F25">
         <v>780</v>
@@ -2358,10 +2358,10 @@
         <v>21</v>
       </c>
       <c r="J25" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="K25" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="L25" t="s">
         <v>24</v>
@@ -2376,10 +2376,10 @@
         <v>26</v>
       </c>
       <c r="P25" s="3" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="Q25" s="3" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="R25">
         <v>4</v>
@@ -2391,15 +2391,15 @@
         <v>1</v>
       </c>
       <c r="U25" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V25" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="B26" t="s">
         <v>17</v>
@@ -2408,10 +2408,10 @@
         <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E26" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F26">
         <v>780</v>
@@ -2423,10 +2423,10 @@
         <v>21</v>
       </c>
       <c r="J26" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="K26" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="L26" t="s">
         <v>24</v>
@@ -2441,10 +2441,10 @@
         <v>26</v>
       </c>
       <c r="P26" s="3" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="Q26" s="3" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="R26">
         <v>4</v>
@@ -2456,15 +2456,15 @@
         <v>1</v>
       </c>
       <c r="U26" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V26" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="B27" t="s">
         <v>17</v>
@@ -2473,10 +2473,10 @@
         <v>24</v>
       </c>
       <c r="D27" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E27" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F27">
         <v>780</v>
@@ -2488,10 +2488,10 @@
         <v>21</v>
       </c>
       <c r="J27" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="K27" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="L27" t="s">
         <v>24</v>
@@ -2506,10 +2506,10 @@
         <v>26</v>
       </c>
       <c r="P27" s="3" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="Q27" s="3" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="R27">
         <v>4</v>
@@ -2521,15 +2521,15 @@
         <v>1</v>
       </c>
       <c r="U27" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V27" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="B28" t="s">
         <v>17</v>
@@ -2538,10 +2538,10 @@
         <v>24</v>
       </c>
       <c r="D28" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E28" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F28">
         <v>780</v>
@@ -2553,10 +2553,10 @@
         <v>21</v>
       </c>
       <c r="J28" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="K28" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="L28" t="s">
         <v>24</v>
@@ -2568,7 +2568,7 @@
         <v>25</v>
       </c>
       <c r="O28" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="P28" s="3" t="s">
         <v>27</v>
@@ -2586,15 +2586,15 @@
         <v>1</v>
       </c>
       <c r="U28" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V28" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="B29" t="s">
         <v>17</v>
@@ -2603,10 +2603,10 @@
         <v>24</v>
       </c>
       <c r="D29" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E29" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F29">
         <v>780</v>
@@ -2618,10 +2618,10 @@
         <v>21</v>
       </c>
       <c r="J29" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="K29" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="L29" t="s">
         <v>24</v>
@@ -2633,10 +2633,10 @@
         <v>25</v>
       </c>
       <c r="O29" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="P29" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Q29" s="3" t="s">
         <v>28</v>
@@ -2651,15 +2651,15 @@
         <v>1</v>
       </c>
       <c r="U29" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V29" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="B30" t="s">
         <v>17</v>
@@ -2668,10 +2668,10 @@
         <v>24</v>
       </c>
       <c r="D30" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E30" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F30">
         <v>780</v>
@@ -2683,10 +2683,10 @@
         <v>21</v>
       </c>
       <c r="J30" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="K30" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="L30" t="s">
         <v>24</v>
@@ -2698,10 +2698,10 @@
         <v>25</v>
       </c>
       <c r="O30" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="P30" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Q30" s="3" t="s">
         <v>28</v>
@@ -2716,15 +2716,15 @@
         <v>1</v>
       </c>
       <c r="U30" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V30" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B31" t="s">
         <v>17</v>
@@ -2733,10 +2733,10 @@
         <v>24</v>
       </c>
       <c r="D31" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="E31" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="F31">
         <v>858</v>
@@ -2745,13 +2745,13 @@
         <v>20</v>
       </c>
       <c r="H31" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="I31" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="J31" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="L31" t="s">
         <v>24</v>
@@ -2763,10 +2763,10 @@
         <v>25</v>
       </c>
       <c r="O31" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="P31" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Q31" s="3" t="s">
         <v>28</v>
@@ -2781,15 +2781,15 @@
         <v>1</v>
       </c>
       <c r="U31" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V31" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="B32" t="s">
         <v>17</v>
@@ -2798,10 +2798,10 @@
         <v>24</v>
       </c>
       <c r="D32" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="E32" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="F32">
         <v>858</v>
@@ -2810,13 +2810,13 @@
         <v>20</v>
       </c>
       <c r="H32" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="I32" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="J32" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="L32" t="s">
         <v>24</v>
@@ -2828,10 +2828,10 @@
         <v>25</v>
       </c>
       <c r="O32" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="P32" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Q32" s="3" t="s">
         <v>28</v>
@@ -2846,15 +2846,15 @@
         <v>1</v>
       </c>
       <c r="U32" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V32" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="B33" t="s">
         <v>17</v>
@@ -2863,10 +2863,10 @@
         <v>24</v>
       </c>
       <c r="D33" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="E33" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="F33">
         <v>858</v>
@@ -2875,13 +2875,13 @@
         <v>20</v>
       </c>
       <c r="H33" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="I33" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="J33" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="L33" t="s">
         <v>24</v>
@@ -2893,7 +2893,7 @@
         <v>25</v>
       </c>
       <c r="O33" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="P33" s="3" t="s">
         <v>27</v>
@@ -2911,15 +2911,15 @@
         <v>1</v>
       </c>
       <c r="U33" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V33" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="B34" t="s">
         <v>17</v>
@@ -2928,10 +2928,10 @@
         <v>24</v>
       </c>
       <c r="D34" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="E34" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="F34">
         <v>858</v>
@@ -2940,13 +2940,13 @@
         <v>20</v>
       </c>
       <c r="H34" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="I34" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="J34" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="L34" t="s">
         <v>24</v>
@@ -2961,10 +2961,10 @@
         <v>26</v>
       </c>
       <c r="P34" s="3" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="Q34" s="3" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="R34">
         <v>2</v>
@@ -2976,15 +2976,15 @@
         <v>1</v>
       </c>
       <c r="U34" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V34" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="B35" t="s">
         <v>17</v>
@@ -2993,10 +2993,10 @@
         <v>24</v>
       </c>
       <c r="D35" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="E35" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="F35">
         <v>858</v>
@@ -3005,13 +3005,13 @@
         <v>20</v>
       </c>
       <c r="H35" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="I35" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="J35" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="L35" t="s">
         <v>24</v>
@@ -3026,10 +3026,10 @@
         <v>26</v>
       </c>
       <c r="P35" s="3" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="Q35" s="3" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="R35">
         <v>2</v>
@@ -3041,15 +3041,15 @@
         <v>1</v>
       </c>
       <c r="U35" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V35" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="B36" t="s">
         <v>17</v>
@@ -3058,10 +3058,10 @@
         <v>24</v>
       </c>
       <c r="D36" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="E36" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="F36">
         <v>858</v>
@@ -3070,13 +3070,13 @@
         <v>20</v>
       </c>
       <c r="H36" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="I36" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="J36" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="L36" t="s">
         <v>24</v>
@@ -3091,7 +3091,7 @@
         <v>26</v>
       </c>
       <c r="P36" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Q36" s="3" t="s">
         <v>28</v>
@@ -3106,15 +3106,15 @@
         <v>1</v>
       </c>
       <c r="U36" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V36" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="B37" t="s">
         <v>17</v>
@@ -3123,10 +3123,10 @@
         <v>24</v>
       </c>
       <c r="D37" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="E37" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="F37">
         <v>858</v>
@@ -3135,13 +3135,13 @@
         <v>20</v>
       </c>
       <c r="H37" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="I37" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="J37" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="L37" t="s">
         <v>24</v>
@@ -3153,10 +3153,10 @@
         <v>25</v>
       </c>
       <c r="O37" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="P37" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Q37" s="3" t="s">
         <v>28</v>
@@ -3171,15 +3171,15 @@
         <v>1</v>
       </c>
       <c r="U37" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V37" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="B38" t="s">
         <v>17</v>
@@ -3188,10 +3188,10 @@
         <v>24</v>
       </c>
       <c r="D38" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="E38" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="F38">
         <v>858</v>
@@ -3200,13 +3200,13 @@
         <v>20</v>
       </c>
       <c r="H38" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="I38" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="J38" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="L38" t="s">
         <v>24</v>
@@ -3218,7 +3218,7 @@
         <v>25</v>
       </c>
       <c r="O38" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="P38" s="3" t="s">
         <v>27</v>
@@ -3236,15 +3236,15 @@
         <v>1</v>
       </c>
       <c r="U38" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V38" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="B39" t="s">
         <v>17</v>
@@ -3253,10 +3253,10 @@
         <v>24</v>
       </c>
       <c r="D39" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="E39" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="F39">
         <v>858</v>
@@ -3265,13 +3265,13 @@
         <v>20</v>
       </c>
       <c r="H39" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="I39" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="J39" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="L39" t="s">
         <v>24</v>
@@ -3283,7 +3283,7 @@
         <v>25</v>
       </c>
       <c r="O39" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="P39" s="3" t="s">
         <v>27</v>
@@ -3301,15 +3301,15 @@
         <v>1</v>
       </c>
       <c r="U39" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V39" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="B40" t="s">
         <v>17</v>
@@ -3318,10 +3318,10 @@
         <v>24</v>
       </c>
       <c r="D40" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="E40" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="F40">
         <v>858</v>
@@ -3330,13 +3330,13 @@
         <v>20</v>
       </c>
       <c r="H40" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="I40" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="J40" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="L40" t="s">
         <v>24</v>
@@ -3348,10 +3348,10 @@
         <v>25</v>
       </c>
       <c r="O40" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="P40" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Q40" s="3" t="s">
         <v>28</v>
@@ -3366,15 +3366,15 @@
         <v>1</v>
       </c>
       <c r="U40" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V40" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="B41" t="s">
         <v>17</v>
@@ -3383,10 +3383,10 @@
         <v>24</v>
       </c>
       <c r="D41" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="E41" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="F41">
         <v>858</v>
@@ -3395,13 +3395,13 @@
         <v>20</v>
       </c>
       <c r="H41" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="I41" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="J41" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="L41" t="s">
         <v>24</v>
@@ -3413,13 +3413,13 @@
         <v>25</v>
       </c>
       <c r="O41" s="3" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="P41" s="3" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="Q41" s="3" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="R41">
         <v>5</v>
@@ -3431,15 +3431,15 @@
         <v>1</v>
       </c>
       <c r="U41" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V41" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="B42" t="s">
         <v>17</v>
@@ -3448,10 +3448,10 @@
         <v>24</v>
       </c>
       <c r="D42" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="E42" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="F42">
         <v>858</v>
@@ -3460,13 +3460,13 @@
         <v>20</v>
       </c>
       <c r="H42" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="I42" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="J42" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="L42" t="s">
         <v>24</v>
@@ -3478,13 +3478,13 @@
         <v>25</v>
       </c>
       <c r="O42" s="3" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="P42" s="3" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="Q42" s="3" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="R42">
         <v>5</v>
@@ -3496,15 +3496,15 @@
         <v>1</v>
       </c>
       <c r="U42" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V42" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="B43" t="s">
         <v>17</v>
@@ -3513,10 +3513,10 @@
         <v>24</v>
       </c>
       <c r="D43" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="E43" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="F43">
         <v>858</v>
@@ -3525,13 +3525,13 @@
         <v>20</v>
       </c>
       <c r="H43" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="I43" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="J43" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="L43" t="s">
         <v>24</v>
@@ -3543,13 +3543,13 @@
         <v>25</v>
       </c>
       <c r="O43" s="3" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="P43" s="3" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="Q43" s="3" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="R43">
         <v>5</v>
@@ -3561,15 +3561,15 @@
         <v>1</v>
       </c>
       <c r="U43" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V43" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>29</v>
+        <v>99</v>
       </c>
       <c r="B44" t="s">
         <v>17</v>
@@ -3626,15 +3626,15 @@
         <v>1</v>
       </c>
       <c r="U44" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V44" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="B45" t="s">
         <v>17</v>
@@ -3691,15 +3691,15 @@
         <v>1</v>
       </c>
       <c r="U45" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V45" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>32</v>
+        <v>101</v>
       </c>
       <c r="B46" t="s">
         <v>17</v>
@@ -3741,7 +3741,7 @@
         <v>26</v>
       </c>
       <c r="P46" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Q46" s="3" t="s">
         <v>28</v>
@@ -3756,15 +3756,15 @@
         <v>1</v>
       </c>
       <c r="U46" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V46" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>34</v>
+        <v>102</v>
       </c>
       <c r="B47" t="s">
         <v>17</v>
@@ -3803,10 +3803,10 @@
         <v>25</v>
       </c>
       <c r="O47" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="P47" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Q47" s="3" t="s">
         <v>28</v>
@@ -3821,15 +3821,15 @@
         <v>1</v>
       </c>
       <c r="U47" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V47" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>35</v>
+        <v>103</v>
       </c>
       <c r="B48" t="s">
         <v>17</v>
@@ -3868,10 +3868,10 @@
         <v>25</v>
       </c>
       <c r="O48" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="P48" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Q48" s="3" t="s">
         <v>28</v>
@@ -3886,15 +3886,15 @@
         <v>1</v>
       </c>
       <c r="U48" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V48" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="B49" t="s">
         <v>17</v>
@@ -3933,7 +3933,7 @@
         <v>25</v>
       </c>
       <c r="O49" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="P49" s="3" t="s">
         <v>27</v>
@@ -3951,15 +3951,15 @@
         <v>1</v>
       </c>
       <c r="U49" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V49" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>38</v>
+        <v>105</v>
       </c>
       <c r="B50" t="s">
         <v>17</v>
@@ -3998,7 +3998,7 @@
         <v>25</v>
       </c>
       <c r="O50" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="P50" s="3" t="s">
         <v>27</v>
@@ -4016,15 +4016,15 @@
         <v>1</v>
       </c>
       <c r="U50" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V50" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>39</v>
+        <v>106</v>
       </c>
       <c r="B51" t="s">
         <v>17</v>
@@ -4063,7 +4063,7 @@
         <v>25</v>
       </c>
       <c r="O51" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="P51" s="3" t="s">
         <v>27</v>
@@ -4081,15 +4081,15 @@
         <v>1</v>
       </c>
       <c r="U51" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V51" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>41</v>
+        <v>107</v>
       </c>
       <c r="B52" t="s">
         <v>17</v>
@@ -4128,7 +4128,7 @@
         <v>25</v>
       </c>
       <c r="O52" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="P52" s="3" t="s">
         <v>27</v>
@@ -4146,15 +4146,15 @@
         <v>1</v>
       </c>
       <c r="U52" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V52" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>42</v>
+        <v>108</v>
       </c>
       <c r="B53" t="s">
         <v>17</v>
@@ -4193,7 +4193,7 @@
         <v>25</v>
       </c>
       <c r="O53" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="P53" s="3" t="s">
         <v>27</v>
@@ -4211,15 +4211,15 @@
         <v>1</v>
       </c>
       <c r="U53" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V53" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>43</v>
+        <v>109</v>
       </c>
       <c r="B54" t="s">
         <v>17</v>
@@ -4258,7 +4258,7 @@
         <v>25</v>
       </c>
       <c r="O54" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="P54" s="3" t="s">
         <v>27</v>
@@ -4276,15 +4276,15 @@
         <v>1</v>
       </c>
       <c r="U54" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V54" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>45</v>
+        <v>110</v>
       </c>
       <c r="B55" t="s">
         <v>17</v>
@@ -4323,7 +4323,7 @@
         <v>25</v>
       </c>
       <c r="O55" s="3" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="P55" s="3" t="s">
         <v>27</v>
@@ -4341,15 +4341,15 @@
         <v>1</v>
       </c>
       <c r="U55" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V55" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>46</v>
+        <v>111</v>
       </c>
       <c r="B56" t="s">
         <v>17</v>
@@ -4388,7 +4388,7 @@
         <v>25</v>
       </c>
       <c r="O56" s="3" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="P56" s="3" t="s">
         <v>27</v>
@@ -4406,10 +4406,10 @@
         <v>1</v>
       </c>
       <c r="U56" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="V56" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>